<commit_message>
Kanhur mesai village result shown to CARD
</commit_message>
<xml_diff>
--- a/PadaliHMSfinal.xlsx
+++ b/PadaliHMSfinal.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishabh\waterbudgeting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8D4EFF-5F44-444F-BC36-33095230F11D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B25E83A-C8F4-42E0-9D85-D6E8F879F32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{72AEDC66-642F-4F7B-B82B-33FB806BBC45}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{72AEDC66-642F-4F7B-B82B-33FB806BBC45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Evaporation</t>
   </si>
@@ -545,7 +546,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -863,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFB5108-50BD-427A-87F0-9E3164A28FEA}">
   <dimension ref="A1:C744"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -9042,4 +9043,318 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B94A8A-E437-4EB2-A741-826FF471E860}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>33</v>
+      </c>
+      <c r="G3">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>39</v>
+      </c>
+      <c r="G5">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>39</v>
+      </c>
+      <c r="G6">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>29</v>
+      </c>
+      <c r="G7">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>28</v>
+      </c>
+      <c r="G8">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>26</v>
+      </c>
+      <c r="G9">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <v>29</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>29</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>28</v>
+      </c>
+      <c r="G13">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>